<commit_message>
inserindo os dados estatistico
</commit_message>
<xml_diff>
--- a/base_agro.xlsx
+++ b/base_agro.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
-  <si>
-    <t>base_agro_atualizada</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>Tipo de Cultivo</t>
   </si>
@@ -149,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -161,13 +158,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -240,29 +248,26 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -285,6 +290,7 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -301,10 +307,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -481,11 +487,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -494,33 +503,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -759,12 +768,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1045,7 +1054,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1316,7 +1325,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1329,452 +1338,441 @@
     <col min="5" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="4">
+        <v>84</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" t="s" s="5">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" t="s" s="5">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" t="s" s="5">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="B7" s="6">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="B8" s="6">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="B9" s="6">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="B13" s="6">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" t="s" s="5">
+        <v>7</v>
+      </c>
+      <c r="B14" s="6">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" t="s" s="5">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="B16" s="6">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s" s="5">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" t="s" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5">
-        <v>84</v>
-      </c>
-      <c r="C3" t="s" s="4">
+      <c r="B17" s="6">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" t="s" s="5">
+        <v>7</v>
+      </c>
+      <c r="B18" s="6">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s" s="5">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="4">
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="B19" s="6">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s" s="5">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="B20" s="6">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" ht="20.05" customHeight="1">
+      <c r="A21" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="B21" s="6">
+        <v>91</v>
+      </c>
+      <c r="C21" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" ht="20.05" customHeight="1">
+      <c r="A22" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" t="s" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="B4" s="7">
-        <v>72</v>
-      </c>
-      <c r="C4" t="s" s="6">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="B5" s="7">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s" s="6">
+      <c r="B23" s="6">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s" s="5">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s" s="5">
         <v>11</v>
       </c>
-      <c r="D5" t="s" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="B6" s="7">
-        <v>92</v>
-      </c>
-      <c r="C6" t="s" s="6">
+    </row>
+    <row r="24" ht="20.05" customHeight="1">
+      <c r="A24" t="s" s="5">
+        <v>4</v>
+      </c>
+      <c r="B24" s="6">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s" s="5">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" ht="20.05" customHeight="1">
+      <c r="A25" t="s" s="5">
+        <v>4</v>
+      </c>
+      <c r="B25" s="6">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s" s="5">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" ht="20.05" customHeight="1">
+      <c r="A26" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="B26" s="6">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s" s="5">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" ht="20.05" customHeight="1">
+      <c r="A27" t="s" s="5">
+        <v>4</v>
+      </c>
+      <c r="B27" s="6">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" ht="20.05" customHeight="1">
+      <c r="A28" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="D6" t="s" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="B7" s="7">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s" s="6">
+      <c r="B28" s="6">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s" s="5">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="D7" t="s" s="6">
+    </row>
+    <row r="29" ht="20.05" customHeight="1">
+      <c r="A29" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="B29" s="6">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s" s="5">
+        <v>39</v>
+      </c>
+      <c r="D29" t="s" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" ht="20.05" customHeight="1">
+      <c r="A30" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="B30" s="6">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" ht="20.05" customHeight="1">
+      <c r="A31" t="s" s="5">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="B8" s="7">
+      <c r="B31" s="6">
         <v>78</v>
       </c>
-      <c r="C8" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="B9" s="7">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s" s="6">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="B10" s="7">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="B11" s="7">
-        <v>96</v>
-      </c>
-      <c r="C11" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="B12" s="7">
-        <v>70</v>
-      </c>
-      <c r="C12" t="s" s="6">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="B13" s="7">
-        <v>57</v>
-      </c>
-      <c r="C13" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="B14" s="7">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="B15" s="7">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="B16" s="7">
-        <v>93</v>
-      </c>
-      <c r="C16" t="s" s="6">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="B17" s="7">
-        <v>60</v>
-      </c>
-      <c r="C17" t="s" s="6">
-        <v>28</v>
-      </c>
-      <c r="D17" t="s" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="B18" s="7">
-        <v>70</v>
-      </c>
-      <c r="C18" t="s" s="6">
-        <v>29</v>
-      </c>
-      <c r="D18" t="s" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="B19" s="7">
-        <v>74</v>
-      </c>
-      <c r="C19" t="s" s="6">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="B20" s="7">
-        <v>78</v>
-      </c>
-      <c r="C20" t="s" s="6">
-        <v>31</v>
-      </c>
-      <c r="D20" t="s" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="B21" s="7">
-        <v>89</v>
-      </c>
-      <c r="C21" t="s" s="6">
-        <v>19</v>
-      </c>
-      <c r="D21" t="s" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="B22" s="7">
-        <v>91</v>
-      </c>
-      <c r="C22" t="s" s="6">
-        <v>32</v>
-      </c>
-      <c r="D22" t="s" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="B23" s="7">
+      <c r="C31" t="s" s="5">
         <v>41</v>
       </c>
-      <c r="C23" t="s" s="6">
-        <v>33</v>
-      </c>
-      <c r="D23" t="s" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="B24" s="7">
-        <v>88</v>
-      </c>
-      <c r="C24" t="s" s="6">
-        <v>34</v>
-      </c>
-      <c r="D24" t="s" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="B25" s="7">
-        <v>45</v>
-      </c>
-      <c r="C25" t="s" s="6">
-        <v>35</v>
-      </c>
-      <c r="D25" t="s" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="B26" s="7">
-        <v>78</v>
-      </c>
-      <c r="C26" t="s" s="6">
-        <v>36</v>
-      </c>
-      <c r="D26" t="s" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="B27" s="7">
-        <v>15</v>
-      </c>
-      <c r="C27" t="s" s="6">
-        <v>37</v>
-      </c>
-      <c r="D27" t="s" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="B28" s="7">
-        <v>17</v>
-      </c>
-      <c r="C28" t="s" s="6">
-        <v>38</v>
-      </c>
-      <c r="D28" t="s" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="B29" s="7">
-        <v>77</v>
-      </c>
-      <c r="C29" t="s" s="6">
-        <v>39</v>
-      </c>
-      <c r="D29" t="s" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="B30" s="7">
-        <v>11</v>
-      </c>
-      <c r="C30" t="s" s="6">
-        <v>40</v>
-      </c>
-      <c r="D30" t="s" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="B31" s="7">
-        <v>24</v>
-      </c>
-      <c r="C31" t="s" s="6">
-        <v>41</v>
-      </c>
-      <c r="D31" t="s" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="B32" s="7">
-        <v>78</v>
-      </c>
-      <c r="C32" t="s" s="6">
-        <v>42</v>
-      </c>
-      <c r="D32" t="s" s="6">
-        <v>7</v>
+      <c r="D31" t="s" s="5">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>